<commit_message>
changes need to be made for conf mat
</commit_message>
<xml_diff>
--- a/Dataset_Tester/Mias_sample.xlsx
+++ b/Dataset_Tester/Mias_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sook Mun\Google Drive\Y3S2\CS2\fit3162\Dataset_Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B3957F-1E77-455B-894B-081604BB747C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E04448-E43D-4B81-ACD8-7BCFACB3FF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="3165" windowWidth="19185" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7155" yWindow="6945" windowWidth="19185" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>mdb001</t>
   </si>
@@ -91,63 +91,6 @@
   </si>
   <si>
     <t>mdb020</t>
-  </si>
-  <si>
-    <t>mdb021</t>
-  </si>
-  <si>
-    <t>mdb022</t>
-  </si>
-  <si>
-    <t>mdb023</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>mdb024</t>
-  </si>
-  <si>
-    <t>mdb025</t>
-  </si>
-  <si>
-    <t>mdb026</t>
-  </si>
-  <si>
-    <t>mdb027</t>
-  </si>
-  <si>
-    <t>mdb028</t>
-  </si>
-  <si>
-    <t>mdb029</t>
-  </si>
-  <si>
-    <t>mdb030</t>
-  </si>
-  <si>
-    <t>mdb031</t>
-  </si>
-  <si>
-    <t>mdb032</t>
-  </si>
-  <si>
-    <t>mdb033</t>
-  </si>
-  <si>
-    <t>mdb034</t>
-  </si>
-  <si>
-    <t>mdb035</t>
-  </si>
-  <si>
-    <t>mdb036</t>
-  </si>
-  <si>
-    <t>mdb037</t>
-  </si>
-  <si>
-    <t>mdb038</t>
   </si>
 </sst>
 </file>
@@ -465,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,150 +584,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix the implementation and re create the prediction model
</commit_message>
<xml_diff>
--- a/Dataset_Tester/Mias_sample.xlsx
+++ b/Dataset_Tester/Mias_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sook Mun\Google Drive\Y3S2\CS2\fit3162\Dataset_Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E04448-E43D-4B81-ACD8-7BCFACB3FF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12B6AE6-ACD1-468C-97D0-74ADB2DDA375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7155" yWindow="6945" windowWidth="19185" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10185" yWindow="3585" windowWidth="19185" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>mdb001</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>mdb020</t>
+  </si>
+  <si>
+    <t>Image_Name</t>
+  </si>
+  <si>
+    <t>Condition</t>
   </si>
 </sst>
 </file>
@@ -408,25 +414,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -434,15 +440,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -450,10 +456,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -582,6 +588,14 @@
       </c>
       <c r="B21" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement input validation for UI
</commit_message>
<xml_diff>
--- a/Dataset_Tester/Mias_sample.xlsx
+++ b/Dataset_Tester/Mias_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sook Mun\Google Drive\Y3S2\CS2\fit3162\Dataset_Tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12B6AE6-ACD1-468C-97D0-74ADB2DDA375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68A4C40-457C-4B48-98B0-3CA4E61FB5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10185" yWindow="3585" windowWidth="19185" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7485" yWindow="2985" windowWidth="19185" windowHeight="10545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>mdb001</t>
   </si>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,14 +590,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>